<commit_message>
only 1 poskyris left
</commit_message>
<xml_diff>
--- a/tyrimas.xlsx
+++ b/tyrimas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivano\Desktop\Magistrinis\LaserCV_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB97690-490B-4748-93AA-2A69E159676A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD11538-3469-41F2-9DAD-4DB785AC9E48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6405" yWindow="975" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,16 +482,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>2.0229436681052402</v>
+        <v>0.97936640865681601</v>
       </c>
       <c r="D6">
-        <v>20.597329924046001</v>
+        <v>3.7735924528225802</v>
       </c>
       <c r="E6">
-        <v>0.1469183</v>
+        <v>0.14646899999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -499,16 +499,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C7">
-        <v>0.97936640865681601</v>
+        <v>0.61367503537374601</v>
       </c>
       <c r="D7">
-        <v>3.7735924528225802</v>
+        <v>8.0622577482985491</v>
       </c>
       <c r="E7">
-        <v>0.14646899999999999</v>
+        <v>0.14398939999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -516,16 +516,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>0.61367503537374601</v>
+        <v>0.26248787031142801</v>
       </c>
       <c r="D8">
-        <v>8.0622577482985491</v>
+        <v>0.76987447698745404</v>
       </c>
       <c r="E8">
-        <v>0.14398939999999999</v>
+        <v>0.1797899</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -533,16 +533,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9">
-        <v>0.26248787031142801</v>
+        <v>0.17433204441147199</v>
       </c>
       <c r="D9">
-        <v>0.76987447698745404</v>
+        <v>0.294520547945197</v>
       </c>
       <c r="E9">
-        <v>0.1797899</v>
+        <v>0.12534300000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -550,16 +550,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10">
-        <v>0.17433204441147199</v>
+        <v>9.7711744135551698E-2</v>
       </c>
       <c r="D10">
-        <v>0.294520547945197</v>
+        <v>0.57575757575757802</v>
       </c>
       <c r="E10">
-        <v>0.12534300000000001</v>
+        <v>0.1378943</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -567,16 +567,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>9.7711744135551698E-2</v>
+        <v>0.15869675698938501</v>
       </c>
       <c r="D11">
-        <v>0.57575757575757802</v>
+        <v>6.4814814814809593E-2</v>
       </c>
       <c r="E11">
-        <v>0.1378943</v>
+        <v>0.1391773</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -584,16 +584,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12">
-        <v>0.15869675698938501</v>
+        <v>1.53979563663623</v>
       </c>
       <c r="D12">
-        <v>6.4814814814809593E-2</v>
+        <v>4.1481481481481497</v>
       </c>
       <c r="E12">
-        <v>0.1391773</v>
+        <v>0.17536740000000001</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -601,16 +601,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>1.53979563663623</v>
+        <v>0.15156997140904099</v>
       </c>
       <c r="D13">
-        <v>4.1481481481481497</v>
+        <v>9.3457943925230297E-2</v>
       </c>
       <c r="E13">
-        <v>0.17536740000000001</v>
+        <v>0.16435449999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -618,16 +618,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14">
-        <v>0.15156997140904099</v>
+        <v>0.151648285813309</v>
       </c>
       <c r="D14">
-        <v>9.3457943925230297E-2</v>
+        <v>2.6119402985074199E-2</v>
       </c>
       <c r="E14">
-        <v>0.16435449999999999</v>
+        <v>0.1797559</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -635,16 +635,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15">
-        <v>0.151648285813309</v>
+        <v>0.69545276946352896</v>
       </c>
       <c r="D15">
-        <v>2.6119402985074199E-2</v>
+        <v>0.954545454545496</v>
       </c>
       <c r="E15">
-        <v>0.1797559</v>
+        <v>0.17295559999999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,16 +652,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C16">
-        <v>5.6947530724769999</v>
+        <v>0.16248989705060499</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2.0750000000000499</v>
       </c>
       <c r="E16">
-        <v>0.1182595</v>
+        <v>0.14608959999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,101 +669,67 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17">
-        <v>0.69545276946352896</v>
+        <v>0.26122514825186699</v>
       </c>
       <c r="D17">
-        <v>0.954545454545496</v>
+        <v>1.0657082490166601</v>
       </c>
       <c r="E17">
-        <v>0.17295559999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>44</v>
-      </c>
-      <c r="C18">
-        <v>0.16248989705060499</v>
-      </c>
-      <c r="D18">
-        <v>2.0750000000000499</v>
-      </c>
-      <c r="E18">
-        <v>0.14608959999999999</v>
+        <v>0.14041790000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>45</v>
+      <c r="B19" t="s">
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>0.26122514825186699</v>
+        <f>MIN(C3:C17)</f>
+        <v>4.2752999999999999E-2</v>
       </c>
       <c r="D19">
-        <v>1.0657082490166601</v>
+        <f>MIN(D3:D17)</f>
+        <v>2.6119402985074199E-2</v>
       </c>
       <c r="E19">
-        <v>0.14041790000000001</v>
+        <f>MIN(E3:E17)</f>
+        <v>0.12534300000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <f>MAX(C3:C17)</f>
+        <v>1.6964174420886</v>
+      </c>
+      <c r="D20">
+        <f>MAX(D3:D17)</f>
+        <v>8.0622577482985491</v>
+      </c>
+      <c r="E20">
+        <f>MAX(E3:E17)</f>
+        <v>0.1797899</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <f>MIN(C3:C19)</f>
-        <v>4.2752999999999999E-2</v>
+        <f>AVERAGE(C3:C17)</f>
+        <v>0.4911418378022423</v>
       </c>
       <c r="D21">
-        <f>MIN(D3:D19)</f>
-        <v>0</v>
+        <f>AVERAGE(D3:D17)</f>
+        <v>1.6871630254074546</v>
       </c>
       <c r="E21">
-        <f>MIN(E3:E19)</f>
-        <v>0.1182595</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22">
-        <f>MAX(C3:C19)</f>
-        <v>5.6947530724769999</v>
-      </c>
-      <c r="D22">
-        <f>MAX(D3:D19)</f>
-        <v>20.597329924046001</v>
-      </c>
-      <c r="E22">
-        <f>MAX(E3:E19)</f>
-        <v>0.1797899</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23">
-        <f>AVERAGE(C3:C19)</f>
-        <v>0.88734260633034556</v>
-      </c>
-      <c r="D23">
-        <f>AVERAGE(D3:D19)</f>
-        <v>2.7002809003034014</v>
-      </c>
-      <c r="E23">
-        <f>AVERAGE(E3:E19)</f>
-        <v>0.15146297647058821</v>
+        <f>AVERAGE(E3:E17)</f>
+        <v>0.15397951999999998</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>